<commit_message>
Pbix com base atualizada
</commit_message>
<xml_diff>
--- a/Arquivos/Dataset/datas_ginasio.xlsx
+++ b/Arquivos/Dataset/datas_ginasio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projeto PP\GymTrend-Task-Force\Arquivos\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ciellos\GymTrendTaskForce\Arquivos\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3FD18E7-41A9-485D-AEF2-23E6A5B7792B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F832562-0283-4827-9340-1ADF7784396C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F1B93DC-92C2-42D1-9A35-581CEBCA38D6}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{2F1B93DC-92C2-42D1-9A35-581CEBCA38D6}"/>
   </bookViews>
   <sheets>
     <sheet name="multiTimeline" sheetId="2" r:id="rId1"/>
@@ -29,10 +29,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -75,6 +75,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="dd/mm/yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,8 +109,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,7 +120,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -455,16 +458,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E522DF5A-2E58-408E-8941-021B224D827D}">
   <dimension ref="A1:C213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,2332 +480,2332 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>44927</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>44927</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>44927</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>44927</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>44934</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>44934</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>44934</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>44934</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C9">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>44941</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>44941</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C11">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>44941</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>44941</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C13">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>44948</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C14">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
         <v>44948</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C15">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>44948</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C16">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>44948</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>44955</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C18">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>44955</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C19">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>44955</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C20">
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>44955</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C21">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>44962</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C22">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>44962</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C23">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>44962</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C24">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>44962</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C25">
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>44969</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C26">
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>44969</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C27">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>44969</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C28">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>44969</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C29">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>44976</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C30">
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>44976</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C31">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>44976</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C32">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>44976</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C33">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>44983</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C34">
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>44983</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C35">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>44983</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C36">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>44983</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C37">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>44990</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C38">
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
         <v>44990</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C39">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
         <v>44990</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C40">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
         <v>44990</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C41">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
         <v>44997</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C42">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>44997</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C43">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
         <v>44997</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C44">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
         <v>44997</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C45">
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>45004</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C46">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>45004</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C47">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>45004</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C48">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <v>45004</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C49">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
         <v>45011</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C50">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <v>45011</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C51">
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>45011</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C52">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
         <v>45011</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C53">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
         <v>45018</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C54">
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
         <v>45018</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C55">
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
         <v>45018</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C56">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
         <v>45018</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C57">
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>45025</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C58">
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
         <v>45025</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C59">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
         <v>45025</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C60">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
         <v>45025</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C61">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
         <v>45032</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C62">
         <v>82</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
         <v>45032</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C63">
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
         <v>45032</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C64">
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
         <v>45032</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C65">
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
         <v>45039</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C66">
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
         <v>45039</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C67">
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
         <v>45039</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C68">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
         <v>45039</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C69">
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
         <v>45046</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C70">
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="1">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
         <v>45046</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C71">
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="1">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
         <v>45046</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C72">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
         <v>45046</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C73">
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
         <v>45053</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C74">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="1">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
         <v>45053</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C75">
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="1">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
         <v>45053</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C76">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="1">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
         <v>45053</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C77">
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="1">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
         <v>45060</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C78">
         <v>64</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
         <v>45060</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C79">
         <v>28</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="1">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
         <v>45060</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C80">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="1">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
         <v>45060</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C81">
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="1">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
         <v>45067</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C82">
         <v>64</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="1">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
         <v>45067</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C83">
         <v>28</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="1">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
         <v>45067</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C84">
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="1">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
         <v>45067</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C85">
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="1">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
         <v>45074</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C86">
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="1">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
         <v>45074</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C87">
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="1">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
         <v>45074</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C88">
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="1">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
         <v>45074</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C89">
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="1">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
         <v>45081</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C90">
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="1">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
         <v>45081</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C91">
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="1">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
         <v>45081</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C92">
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="1">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
         <v>45081</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C93">
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="1">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
         <v>45088</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C94">
         <v>86</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="1">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
         <v>45088</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C95">
         <v>27</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="1">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
         <v>45088</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C96">
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="1">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
         <v>45088</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C97">
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="1">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
         <v>45095</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C98">
         <v>85</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="1">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
         <v>45095</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C99">
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="1">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
         <v>45095</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C100">
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="1">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
         <v>45095</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C101">
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="1">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
         <v>45102</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B102" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C102">
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="1">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
         <v>45102</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B103" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C103">
         <v>35</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="1">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
         <v>45102</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C104">
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="1">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
         <v>45102</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C105">
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="1">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
         <v>45109</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C106">
         <v>91</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="1">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
         <v>45109</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C107">
         <v>30</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="1">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
         <v>45109</v>
       </c>
-      <c r="B108" s="2" t="s">
+      <c r="B108" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C108">
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="1">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
         <v>45109</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B109" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C109">
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="1">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
         <v>45116</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B110" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C110">
         <v>79</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="1">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
         <v>45116</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C111">
         <v>29</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="1">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
         <v>45116</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B112" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C112">
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="1">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
         <v>45116</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C113">
         <v>9</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="1">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
         <v>45123</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C114">
         <v>64</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="1">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
         <v>45123</v>
       </c>
-      <c r="B115" s="2" t="s">
+      <c r="B115" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C115">
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="1">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
         <v>45123</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C116">
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" s="1">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
         <v>45123</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C117">
         <v>9</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="1">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
         <v>45130</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C118">
         <v>64</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="1">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
         <v>45130</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B119" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C119">
         <v>27</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" s="1">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
         <v>45130</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C120">
         <v>3</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" s="1">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
         <v>45130</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C121">
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" s="1">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
         <v>45137</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C122">
         <v>80</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="1">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
         <v>45137</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C123">
         <v>28</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" s="1">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
         <v>45137</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B124" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C124">
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="1">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
         <v>45137</v>
       </c>
-      <c r="B125" s="2" t="s">
+      <c r="B125" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C125">
         <v>10</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="1">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
         <v>45144</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B126" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C126">
         <v>63</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" s="1">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
         <v>45144</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C127">
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="1">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
         <v>45144</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="B128" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C128">
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="1">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="2">
         <v>45144</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B129" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C129">
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="1">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
         <v>45151</v>
       </c>
-      <c r="B130" s="2" t="s">
+      <c r="B130" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C130">
         <v>71</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" s="1">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
         <v>45151</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C131">
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" s="1">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
         <v>45151</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="B132" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C132">
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" s="1">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
         <v>45151</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B133" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C133">
         <v>14</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" s="1">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
         <v>45158</v>
       </c>
-      <c r="B134" s="2" t="s">
+      <c r="B134" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C134">
         <v>86</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" s="1">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
         <v>45158</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C135">
         <v>29</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" s="1">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
         <v>45158</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C136">
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" s="1">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="2">
         <v>45158</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B137" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C137">
         <v>14</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" s="1">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
         <v>45165</v>
       </c>
-      <c r="B138" s="2" t="s">
+      <c r="B138" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C138">
         <v>77</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" s="1">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
         <v>45165</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B139" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C139">
         <v>29</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" s="1">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
         <v>45165</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="B140" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C140">
         <v>9</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" s="1">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
         <v>45165</v>
       </c>
-      <c r="B141" s="2" t="s">
+      <c r="B141" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C141">
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" s="1">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
         <v>45172</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B142" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C142">
         <v>97</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" s="1">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
         <v>45172</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B143" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C143">
         <v>41</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" s="1">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
         <v>45172</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B144" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C144">
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" s="1">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="2">
         <v>45172</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B145" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C145">
         <v>20</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="1">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
         <v>45179</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B146" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C146">
         <v>93</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" s="1">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
         <v>45179</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B147" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C147">
         <v>39</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="1">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
         <v>45179</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B148" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C148">
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" s="1">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
         <v>45179</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B149" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C149">
         <v>20</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" s="1">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
         <v>45186</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B150" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C150">
         <v>85</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" s="1">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
         <v>45186</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B151" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C151">
         <v>33</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" s="1">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
         <v>45186</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B152" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C152">
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" s="1">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="2">
         <v>45186</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B153" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C153">
         <v>14</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" s="1">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
         <v>45193</v>
       </c>
-      <c r="B154" s="2" t="s">
+      <c r="B154" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C154">
         <v>81</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" s="1">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
         <v>45193</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B155" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C155">
         <v>30</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" s="1">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
         <v>45193</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B156" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C156">
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" s="1">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
         <v>45193</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B157" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C157">
         <v>13</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" s="1">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
         <v>45200</v>
       </c>
-      <c r="B158" s="2" t="s">
+      <c r="B158" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C158">
         <v>83</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" s="1">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
         <v>45200</v>
       </c>
-      <c r="B159" s="2" t="s">
+      <c r="B159" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C159">
         <v>32</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" s="1">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
         <v>45200</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B160" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C160">
         <v>7</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" s="1">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="2">
         <v>45200</v>
       </c>
-      <c r="B161" s="2" t="s">
+      <c r="B161" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C161">
         <v>14</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="1">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
         <v>45207</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B162" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C162">
         <v>77</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" s="1">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
         <v>45207</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B163" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C163">
         <v>28</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164" s="1">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
         <v>45207</v>
       </c>
-      <c r="B164" s="2" t="s">
+      <c r="B164" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C164">
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" s="1">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
         <v>45207</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="B165" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C165">
         <v>13</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" s="1">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
         <v>45214</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="B166" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C166">
         <v>74</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" s="1">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
         <v>45214</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B167" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C167">
         <v>33</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A168" s="1">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
         <v>45214</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B168" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C168">
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" s="1">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="2">
         <v>45214</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="B169" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C169">
         <v>11</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170" s="1">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
         <v>45221</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="B170" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C170">
         <v>72</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A171" s="1">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
         <v>45221</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B171" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C171">
         <v>21</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A172" s="1">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
         <v>45221</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B172" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C172">
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A173" s="1">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
         <v>45221</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B173" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C173">
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A174" s="1">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
         <v>45228</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B174" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C174">
         <v>72</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" s="1">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
         <v>45228</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B175" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C175">
         <v>22</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176" s="1">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
         <v>45228</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="B176" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C176">
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A177" s="1">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
         <v>45228</v>
       </c>
-      <c r="B177" s="2" t="s">
+      <c r="B177" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C177">
         <v>16</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A178" s="1">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
         <v>45235</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="B178" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C178">
         <v>68</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" s="1">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
         <v>45235</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B179" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C179">
         <v>24</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180" s="1">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
         <v>45235</v>
       </c>
-      <c r="B180" s="2" t="s">
+      <c r="B180" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C180">
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A181" s="1">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
         <v>45235</v>
       </c>
-      <c r="B181" s="2" t="s">
+      <c r="B181" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C181">
         <v>14</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A182" s="1">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
         <v>45242</v>
       </c>
-      <c r="B182" s="2" t="s">
+      <c r="B182" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C182">
         <v>68</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183" s="1">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
         <v>45242</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B183" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C183">
         <v>27</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A184" s="1">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
         <v>45242</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C184">
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A185" s="1">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
         <v>45242</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B185" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C185">
         <v>15</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186" s="1">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
         <v>45249</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B186" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C186">
         <v>62</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A187" s="1">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
         <v>45249</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B187" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C187">
         <v>20</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A188" s="1">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
         <v>45249</v>
       </c>
-      <c r="B188" s="2" t="s">
+      <c r="B188" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C188">
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A189" s="1">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
         <v>45249</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="B189" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C189">
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A190" s="1">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
         <v>45256</v>
       </c>
-      <c r="B190" s="2" t="s">
+      <c r="B190" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C190">
         <v>66</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A191" s="1">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
         <v>45256</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B191" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C191">
         <v>29</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A192" s="1">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
         <v>45256</v>
       </c>
-      <c r="B192" s="2" t="s">
+      <c r="B192" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C192">
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" s="1">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
         <v>45256</v>
       </c>
-      <c r="B193" s="2" t="s">
+      <c r="B193" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C193">
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" s="1">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
         <v>45263</v>
       </c>
-      <c r="B194" s="2" t="s">
+      <c r="B194" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C194">
         <v>68</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" s="1">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
         <v>45263</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="B195" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C195">
         <v>28</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" s="1">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
         <v>45263</v>
       </c>
-      <c r="B196" s="2" t="s">
+      <c r="B196" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C196">
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" s="1">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
         <v>45263</v>
       </c>
-      <c r="B197" s="2" t="s">
+      <c r="B197" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C197">
         <v>8</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A198" s="1">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
         <v>45270</v>
       </c>
-      <c r="B198" s="2" t="s">
+      <c r="B198" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C198">
         <v>60</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A199" s="1">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
         <v>45270</v>
       </c>
-      <c r="B199" s="2" t="s">
+      <c r="B199" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C199">
         <v>26</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" s="1">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
         <v>45270</v>
       </c>
-      <c r="B200" s="2" t="s">
+      <c r="B200" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C200">
         <v>6</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201" s="1">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
         <v>45270</v>
       </c>
-      <c r="B201" s="2" t="s">
+      <c r="B201" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C201">
         <v>8</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202" s="1">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
         <v>45277</v>
       </c>
-      <c r="B202" s="2" t="s">
+      <c r="B202" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C202">
         <v>57</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A203" s="1">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
         <v>45277</v>
       </c>
-      <c r="B203" s="2" t="s">
+      <c r="B203" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C203">
         <v>22</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A204" s="1">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
         <v>45277</v>
       </c>
-      <c r="B204" s="2" t="s">
+      <c r="B204" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C204">
         <v>3</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A205" s="1">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
         <v>45277</v>
       </c>
-      <c r="B205" s="2" t="s">
+      <c r="B205" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C205">
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A206" s="1">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
         <v>45284</v>
       </c>
-      <c r="B206" s="2" t="s">
+      <c r="B206" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C206">
         <v>67</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A207" s="1">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
         <v>45284</v>
       </c>
-      <c r="B207" s="2" t="s">
+      <c r="B207" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C207">
         <v>19</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A208" s="1">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
         <v>45284</v>
       </c>
-      <c r="B208" s="2" t="s">
+      <c r="B208" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C208">
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A209" s="1">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" s="2">
         <v>45284</v>
       </c>
-      <c r="B209" s="2" t="s">
+      <c r="B209" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C209">
         <v>11</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A210" s="1">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
         <v>45291</v>
       </c>
-      <c r="B210" s="2" t="s">
+      <c r="B210" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C210">
         <v>97</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A211" s="1">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
         <v>45291</v>
       </c>
-      <c r="B211" s="2" t="s">
+      <c r="B211" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C211">
         <v>42</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A212" s="1">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
         <v>45291</v>
       </c>
-      <c r="B212" s="2" t="s">
+      <c r="B212" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C212">
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A213" s="1">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
         <v>45291</v>
       </c>
-      <c r="B213" s="2" t="s">
+      <c r="B213" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C213">
@@ -2809,8 +2814,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2821,7 +2827,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>